<commit_message>
Versión 1.5 manual, se agregan formatos
</commit_message>
<xml_diff>
--- a/05 INVENTARIOS/SISTEMAS/inventario.xlsx
+++ b/05 INVENTARIOS/SISTEMAS/inventario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Trabajo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Recepcion Reforma\Documents\CONSERVACION\05 INVENTARIOS\SISTEMAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95C2A8A-A181-46E0-8E03-C9B818E5197B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2EBB00-852B-45F7-8F2F-EB2D7E3B6B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{BAB93A1A-43F8-4E5A-8969-275C58EA17A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{BAB93A1A-43F8-4E5A-8969-275C58EA17A3}"/>
   </bookViews>
   <sheets>
     <sheet name="MÁQUINAS" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>TPC-Q003</t>
   </si>
   <si>
-    <t>4CS120RGD</t>
-  </si>
-  <si>
     <t>Alimentación / Conector</t>
   </si>
   <si>
@@ -387,6 +384,9 @@
   </si>
   <si>
     <t>VND3R72440</t>
+  </si>
+  <si>
+    <t>4CS1260RGD</t>
   </si>
 </sst>
 </file>
@@ -483,15 +483,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -508,6 +499,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -961,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E00E46-5D25-4F0E-86C4-641767DDD438}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,7 +993,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -1008,15 +1008,15 @@
         <v>7</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
@@ -1024,54 +1024,54 @@
       <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>38</v>
+        <v>114</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>42</v>
+      <c r="F3" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
@@ -1080,109 +1080,109 @@
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>44</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>42</v>
+        <v>57</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>55</v>
+        <v>64</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>12</v>
@@ -1191,13 +1191,13 @@
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>38</v>
+      <c r="F8" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -1755,7 +1755,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="6" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="1"/>
     <col min="4" max="4" width="28.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="30.42578125" style="2" customWidth="1"/>
@@ -1763,10 +1763,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1782,111 +1782,111 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="A2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>55</v>
+      <c r="F2" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H2" s="2">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>60</v>
+      <c r="A3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>53</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H3" s="2">
         <v>18.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>55</v>
+      <c r="F4" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" s="2">
         <v>19.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="10">
+      <c r="A5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="7">
         <v>0.67291666666666661</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>55</v>
+      <c r="F5" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1913,12 +1913,12 @@
     <col min="1" max="1" width="15.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="1"/>
     <col min="3" max="3" width="12.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="41.42578125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" style="6" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1927,153 +1927,153 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>82</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>91</v>
+        <v>108</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>95</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2088,7 +2088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD083357-E7CF-48B5-A44C-59E9596C1994}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -2103,111 +2103,111 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2"/>
       <c r="E2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D3"/>
       <c r="E3" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4"/>
       <c r="E4" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="D6"/>
       <c r="E6" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -2227,81 +2227,81 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="H2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="5"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+      <c r="H2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>